<commit_message>
chapter 4 assessment 2
</commit_message>
<xml_diff>
--- a/AssessmentAnswers.xlsx
+++ b/AssessmentAnswers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB01E2D-962D-4DAB-AF38-9BAD9C994DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0EFB75-4EB5-468E-91DB-2E07264C05D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{DF2722FF-B284-4057-B8C2-DC8A19C58944}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -1786,86 +1786,131 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED693C8-FD51-4782-AB42-89326B96C028}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chapter 11 review yipeeeeee :D
</commit_message>
<xml_diff>
--- a/AssessmentAnswers.xlsx
+++ b/AssessmentAnswers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813EB5A4-B855-4D4A-9D9F-26E099D1C35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D140DC4-A942-4C89-8FCD-B1C2E36BE32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="12" xr2:uid="{DF2722FF-B284-4057-B8C2-DC8A19C58944}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -1686,7 +1686,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="B15" sqref="B1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,15 +1818,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BEC2C6-547D-421C-82EF-3F043331E1DC}">
-  <dimension ref="A1:AC15"/>
+  <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1887,8 +1887,14 @@
       <c r="AC1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1949,8 +1955,14 @@
       <c r="AC2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2011,8 +2023,14 @@
       <c r="AC3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2073,8 +2091,14 @@
       <c r="AC4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2135,8 +2159,14 @@
       <c r="AC5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2197,8 +2227,14 @@
       <c r="AC6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2259,8 +2295,14 @@
       <c r="AC7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2321,8 +2363,14 @@
       <c r="AC8" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2383,8 +2431,14 @@
       <c r="AC9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2445,8 +2499,14 @@
       <c r="AC10" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2507,8 +2567,14 @@
       <c r="AC11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2569,8 +2635,14 @@
       <c r="AC12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2631,8 +2703,14 @@
       <c r="AC13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2693,8 +2771,14 @@
       <c r="AC14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AE14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2754,6 +2838,12 @@
       </c>
       <c r="AC15" t="s">
         <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pre assessment 2nd try
</commit_message>
<xml_diff>
--- a/AssessmentAnswers.xlsx
+++ b/AssessmentAnswers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\OneDrive\Documents\Projects\security-plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D140DC4-A942-4C89-8FCD-B1C2E36BE32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF14760-21EC-4FA5-AF28-21190AD808F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="12" xr2:uid="{DF2722FF-B284-4057-B8C2-DC8A19C58944}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="13" xr2:uid="{DF2722FF-B284-4057-B8C2-DC8A19C58944}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre assessment first try" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="Chapter 10" sheetId="11" r:id="rId11"/>
     <sheet name="Chapter 11" sheetId="12" r:id="rId12"/>
     <sheet name="Review" sheetId="13" r:id="rId13"/>
+    <sheet name="Pre-assessment 2" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet2" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -488,7 +490,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BEC2C6-547D-421C-82EF-3F043331E1DC}">
   <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
@@ -2847,6 +2849,937 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A573059E-97BB-4F92-ADF0-FE4F12003AC6}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="str">
+        <f>IF(A1=B1, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+      <c r="D1">
+        <f>COUNTIF(C:C, "Correct") / (COUNTIF(C:C, "Correct") + COUNTIF(C:C, "Incorrect"))</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">IF(A2=B2, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C75" si="1">IF(A66=B66, "Correct", "Incorrect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>Incorrect</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F213327-9097-46D0-9C97-7A6936087FE3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>